<commit_message>
Changed gradient colors, white teal colors, and changed white definition to look more white through the keycaps
</commit_message>
<xml_diff>
--- a/Notes and scripts/Alt layout help sheet.xlsx
+++ b/Notes and scripts/Alt layout help sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liam2/Documents/GitHub/qmk_firmware/Notes and scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA61007B-419E-084F-9866-8FBE1C382465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87587DEE-F709-5E41-88AA-DCF96ED1838D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{A6F6E149-121B-F84A-9B42-431FA814CB94}"/>
+    <workbookView xWindow="38380" yWindow="-2780" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{A6F6E149-121B-F84A-9B42-431FA814CB94}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone map" sheetId="1" r:id="rId1"/>
@@ -1606,8 +1606,8 @@
   </sheetPr>
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1661,43 +1661,43 @@
     </row>
     <row r="2" spans="1:17" ht="25" customHeight="1">
       <c r="B2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N2" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="11" customFormat="1">
@@ -1755,10 +1755,10 @@
     </row>
     <row r="4" spans="1:17" ht="25" customHeight="1">
       <c r="A4" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="14">
         <v>2</v>
@@ -1797,13 +1797,13 @@
         <v>2</v>
       </c>
       <c r="O4" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P4" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="11" customFormat="1">
@@ -1861,40 +1861,40 @@
     </row>
     <row r="6" spans="1:17" ht="25" customHeight="1">
       <c r="A6" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
       </c>
       <c r="C6" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L6" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M6" s="14">
         <v>2</v>
@@ -1903,13 +1903,13 @@
         <v>2</v>
       </c>
       <c r="O6" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P6" s="14">
         <v>2</v>
       </c>
       <c r="Q6" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="11" customFormat="1">
@@ -1965,53 +1965,53 @@
     </row>
     <row r="8" spans="1:17" ht="25" customHeight="1">
       <c r="A8" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="14">
         <v>1</v>
       </c>
       <c r="C8" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K8" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L8" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M8" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N8" s="16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="14">
         <v>2</v>
       </c>
       <c r="Q8" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="11" customFormat="1">
@@ -2067,44 +2067,44 @@
     </row>
     <row r="10" spans="1:17" ht="25" customHeight="1">
       <c r="A10" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="22">
         <v>1</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H10" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I10" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J10" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K10" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L10" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M10" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N10" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O10" s="14">
         <v>1</v>
@@ -2113,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="Q10" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="11" customFormat="1">
@@ -2159,19 +2159,19 @@
     </row>
     <row r="12" spans="1:17" ht="25" customHeight="1">
       <c r="A12" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -2180,10 +2180,10 @@
       <c r="J12" s="17"/>
       <c r="K12" s="18"/>
       <c r="L12" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N12" s="14">
         <v>1</v>
@@ -2195,7 +2195,7 @@
         <v>1</v>
       </c>
       <c r="Q12" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2247,49 +2247,49 @@
     </row>
     <row r="14" spans="1:17" ht="25" customHeight="1">
       <c r="B14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="25" customHeight="1"/>
@@ -2324,7 +2324,7 @@
   <dimension ref="A1:K107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="B3">
         <f>Layout!B4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2397,11 +2397,11 @@
       </c>
       <c r="F3">
         <f>COUNTIF($B3,F$2)*POWER(2,$D3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:K3" si="0">COUNTIF($B3,G$2)*POWER(2,$D3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" si="0"/>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="B16">
         <f ca="1">OFFSET(Layout!$B$4,0,13)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="1"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="1"/>
@@ -2933,7 +2933,7 @@
       </c>
       <c r="B17">
         <f ca="1">OFFSET(Layout!$B$4,0,14)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="1"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="1"/>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B19">
         <f ca="1">OFFSET(Layout!$B$6,0,1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3021,15 +3021,15 @@
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="1"/>
         <v>65536</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="B20">
         <f ca="1">OFFSET(Layout!$B$6,0,2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3060,15 +3060,15 @@
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="1"/>
         <v>131072</v>
-      </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="B21">
         <f ca="1">OFFSET(Layout!$B$6,0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3099,15 +3099,15 @@
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="1"/>
         <v>262144</v>
-      </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="B22">
         <f ca="1">OFFSET(Layout!$B$6,0,4)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>524288</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="1"/>
-        <v>524288</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="1"/>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B23">
         <f ca="1">OFFSET(Layout!$B$6,0,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1048576</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="1"/>
-        <v>1048576</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="1"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B24">
         <f ca="1">OFFSET(Layout!$B$6,0,6)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2097152</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
@@ -3232,7 +3232,7 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="1"/>
-        <v>2097152</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="1"/>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B25">
         <f ca="1">OFFSET(Layout!$B$6,0,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4194304</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="1"/>
-        <v>4194304</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="1"/>
@@ -3284,7 +3284,7 @@
       </c>
       <c r="B26">
         <f ca="1">OFFSET(Layout!$B$6,0,8)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3302,7 +3302,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8388608</v>
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="1"/>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="1"/>
-        <v>8388608</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="1"/>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="B27">
         <f ca="1">OFFSET(Layout!$B$6,0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>16777216</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="1"/>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="J27">
         <f t="shared" ca="1" si="1"/>
-        <v>16777216</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="1"/>
@@ -3362,7 +3362,7 @@
       </c>
       <c r="B28">
         <f ca="1">OFFSET(Layout!$B$6,0,10)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>33554432</v>
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="1"/>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="J28">
         <f t="shared" ca="1" si="1"/>
-        <v>33554432</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="1"/>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="B31">
         <f ca="1">OFFSET(Layout!$B$6,0,13)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>268435456</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="J31">
         <f t="shared" ca="1" si="1"/>
-        <v>268435456</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="1"/>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="B34">
         <f ca="1">OFFSET(Layout!$B$8,0,1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3606,15 +3606,15 @@
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ca="1" si="1"/>
         <v>2147483648</v>
-      </c>
-      <c r="G34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="1"/>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="B35">
         <f ca="1">OFFSET(Layout!$B$8,0,2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="1"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="1"/>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="B36">
         <f ca="1">OFFSET(Layout!$B$8,0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36">
         <f t="shared" ca="1" si="1"/>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B37">
         <f ca="1">OFFSET(Layout!$B$8,0,4)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="1"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="J37">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="1"/>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="B38">
         <f ca="1">OFFSET(Layout!$B$8,0,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="1"/>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="J38">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="1"/>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="B39">
         <f ca="1">OFFSET(Layout!$B$8,0,6)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="1"/>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="J39">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="1"/>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="B40">
         <f ca="1">OFFSET(Layout!$B$8,0,7)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="1"/>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="J40">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="1"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B41">
         <f ca="1">OFFSET(Layout!$B$8,0,8)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="1"/>
@@ -3895,7 +3895,7 @@
       </c>
       <c r="J41">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="K41">
         <f t="shared" ca="1" si="1"/>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="B42">
         <f ca="1">OFFSET(Layout!$B$8,0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="H42">
         <f t="shared" ref="G42:K57" ca="1" si="3">COUNTIF($B42,H$2)*POWER(2,$D42)</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="3"/>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="J42">
         <f t="shared" ca="1" si="3"/>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="3"/>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="B43">
         <f ca="1">OFFSET(Layout!$B$8,0,10)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="3"/>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J43">
         <f t="shared" ca="1" si="3"/>
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="3"/>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="B44">
         <f ca="1">OFFSET(Layout!$B$8,0,11)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -4000,7 +4000,7 @@
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="3"/>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="J44">
         <f t="shared" ca="1" si="3"/>
-        <v>512</v>
+        <v>0</v>
       </c>
       <c r="K44">
         <f t="shared" ca="1" si="3"/>
@@ -4025,7 +4025,7 @@
       </c>
       <c r="B45">
         <f>Layout!N8</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="G45">
         <f t="shared" si="3"/>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="I45">
         <f t="shared" si="3"/>
-        <v>1024</v>
+        <v>0</v>
       </c>
       <c r="J45">
         <f t="shared" si="3"/>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="B48">
         <f>Layout!D10</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -4152,7 +4152,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="1"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <f t="shared" si="3"/>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="H48">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="I48">
         <f t="shared" si="3"/>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B49">
         <f ca="1">OFFSET(Layout!$D$10,0,1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="3"/>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="3"/>
@@ -4220,7 +4220,7 @@
       </c>
       <c r="B50">
         <f ca="1">OFFSET(Layout!$D$10,0,2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="3"/>
@@ -4238,7 +4238,7 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="3"/>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="B51">
         <f ca="1">OFFSET(Layout!$D$10,0,3)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -4277,7 +4277,7 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>65536</v>
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="3"/>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="J51">
         <f t="shared" ca="1" si="3"/>
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="3"/>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="B52">
         <f ca="1">OFFSET(Layout!$D$10,0,4)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>131072</v>
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="3"/>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="J52">
         <f t="shared" ca="1" si="3"/>
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="3"/>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="B53">
         <f ca="1">OFFSET(Layout!$D$10,0,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -4355,7 +4355,7 @@
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>262144</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="3"/>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="J53">
         <f t="shared" ca="1" si="3"/>
-        <v>262144</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="3"/>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="B54">
         <f ca="1">OFFSET(Layout!$D$10,0,6)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>2</v>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>524288</v>
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="3"/>
@@ -4402,7 +4402,7 @@
       </c>
       <c r="J54">
         <f t="shared" ca="1" si="3"/>
-        <v>524288</v>
+        <v>0</v>
       </c>
       <c r="K54">
         <f t="shared" ca="1" si="3"/>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="B55">
         <f ca="1">OFFSET(Layout!$D$10,0,7)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1048576</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="3"/>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="J55">
         <f t="shared" ca="1" si="3"/>
-        <v>1048576</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="3"/>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="B56">
         <f ca="1">OFFSET(Layout!$D$10,0,8)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2097152</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="3"/>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="J56">
         <f t="shared" ca="1" si="3"/>
-        <v>2097152</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="3"/>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="B57">
         <f ca="1">OFFSET(Layout!$D$10,0,9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4194304</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="3"/>
@@ -4519,7 +4519,7 @@
       </c>
       <c r="J57">
         <f t="shared" ca="1" si="3"/>
-        <v>4194304</v>
+        <v>0</v>
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="3"/>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="B58">
         <f ca="1">OFFSET(Layout!$D$10,0,10)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8388608</v>
       </c>
       <c r="G58">
         <f t="shared" ref="G58:K67" ca="1" si="4">COUNTIF($B58,G$2)*POWER(2,$D58)</f>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="J58">
         <f t="shared" ca="1" si="4"/>
-        <v>8388608</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="4"/>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="B61">
         <f>Layout!B12</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -4659,7 +4659,7 @@
       </c>
       <c r="F61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>67108864</v>
       </c>
       <c r="G61">
         <f t="shared" si="4"/>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="J61">
         <f t="shared" si="4"/>
-        <v>67108864</v>
+        <v>0</v>
       </c>
       <c r="K61">
         <f t="shared" si="4"/>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="B62">
         <f>Layout!C12</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -4698,7 +4698,7 @@
       </c>
       <c r="F62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>134217728</v>
       </c>
       <c r="G62">
         <f t="shared" si="4"/>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="J62">
         <f t="shared" si="4"/>
-        <v>134217728</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <f t="shared" si="4"/>
@@ -4727,7 +4727,7 @@
       </c>
       <c r="B63">
         <f>Layout!D12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -4737,11 +4737,11 @@
       </c>
       <c r="F63">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>268435456</v>
       </c>
       <c r="G63">
         <f t="shared" si="4"/>
-        <v>268435456</v>
+        <v>0</v>
       </c>
       <c r="H63">
         <f t="shared" si="4"/>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="B64">
         <f>Layout!E12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -4776,11 +4776,11 @@
       </c>
       <c r="F64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>536870912</v>
       </c>
       <c r="G64">
         <f t="shared" si="4"/>
-        <v>536870912</v>
+        <v>0</v>
       </c>
       <c r="H64">
         <f t="shared" si="4"/>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="B65">
         <f>Layout!L12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -4815,11 +4815,11 @@
       </c>
       <c r="F65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1073741824</v>
       </c>
       <c r="G65">
         <f t="shared" si="4"/>
-        <v>1073741824</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <f t="shared" si="4"/>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="B66">
         <f ca="1">OFFSET(Layout!$L$12,0,1)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2147483648</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="4"/>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="4"/>
-        <v>2147483648</v>
+        <v>0</v>
       </c>
       <c r="J66">
         <f t="shared" ca="1" si="4"/>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="B70">
         <f>Layout!B14</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70">
         <v>3</v>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="F70">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G70">
         <f t="shared" si="5"/>
@@ -5018,7 +5018,7 @@
       </c>
       <c r="H70">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I70">
         <f t="shared" si="5"/>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="B71">
         <f ca="1">OFFSET(Layout!$B$14,0,1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="5"/>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="5"/>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="B72">
         <f ca="1">OFFSET(Layout!$B$14,0,2)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="5"/>
@@ -5096,7 +5096,7 @@
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="5"/>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B73">
         <f ca="1">OFFSET(Layout!$B$14,0,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C73">
         <v>3</v>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="5"/>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="5"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="5"/>
@@ -5156,7 +5156,7 @@
       </c>
       <c r="B74">
         <f ca="1">OFFSET(Layout!$B$14,0,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="5"/>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="5"/>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="5"/>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="B75">
         <f ca="1">OFFSET(Layout!$B$14,0,5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75">
         <v>3</v>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="5"/>
@@ -5213,7 +5213,7 @@
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="5"/>
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="5"/>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="B76">
         <f ca="1">OFFSET(Layout!$B$14,0,6)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="5"/>
@@ -5252,7 +5252,7 @@
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="5"/>
-        <v>512</v>
+        <v>0</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="5"/>
@@ -5273,7 +5273,7 @@
       </c>
       <c r="B77">
         <f ca="1">OFFSET(Layout!$B$14,0,7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C77">
         <v>3</v>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="5"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="5"/>
-        <v>1024</v>
+        <v>0</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="5"/>
@@ -5312,7 +5312,7 @@
       </c>
       <c r="B78">
         <f ca="1">OFFSET(Layout!$B$14,0,8)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>2048</v>
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="5"/>
@@ -5330,7 +5330,7 @@
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="5"/>
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="5"/>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="B79">
         <f ca="1">OFFSET(Layout!$B$14,0,9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="5"/>
@@ -5369,7 +5369,7 @@
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="5"/>
-        <v>4096</v>
+        <v>0</v>
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="5"/>
@@ -5390,7 +5390,7 @@
       </c>
       <c r="B80">
         <f ca="1">OFFSET(Layout!$B$14,0,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -5400,7 +5400,7 @@
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="5"/>
@@ -5408,7 +5408,7 @@
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="5"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="5"/>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="B81">
         <f ca="1">OFFSET(Layout!$B$14,0,11)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="5"/>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="5"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="5"/>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="B82">
         <f ca="1">OFFSET(Layout!$B$14,0,12)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>3</v>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="F82">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="5"/>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="5"/>
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="5"/>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B83">
         <f ca="1">OFFSET(Layout!$B$14,0,13)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>3</v>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>65536</v>
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="5"/>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="5"/>
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="5"/>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="B84">
         <f ca="1">OFFSET(Layout!$B$14,0,14)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -5556,7 +5556,7 @@
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>131072</v>
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="5"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="5"/>
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="5"/>
@@ -5585,7 +5585,7 @@
       </c>
       <c r="B85">
         <f>Layout!Q12</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="F85">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>262144</v>
       </c>
       <c r="G85">
         <f t="shared" si="5"/>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="H85">
         <f t="shared" si="5"/>
-        <v>262144</v>
+        <v>0</v>
       </c>
       <c r="I85">
         <f t="shared" si="5"/>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="B86">
         <f ca="1">OFFSET(Layout!$Q$12,-2,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>524288</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="5"/>
@@ -5642,7 +5642,7 @@
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="5"/>
-        <v>524288</v>
+        <v>0</v>
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="5"/>
@@ -5663,7 +5663,7 @@
       </c>
       <c r="B87">
         <f ca="1">OFFSET(Layout!$Q$12,-4,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>3</v>
@@ -5673,7 +5673,7 @@
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1048576</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="5"/>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="5"/>
-        <v>1048576</v>
+        <v>0</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="5"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="B88">
         <f ca="1">OFFSET(Layout!$Q$12,-6,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -5712,7 +5712,7 @@
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>2097152</v>
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="5"/>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="5"/>
-        <v>2097152</v>
+        <v>0</v>
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="5"/>
@@ -5741,7 +5741,7 @@
       </c>
       <c r="B89">
         <f ca="1">OFFSET(Layout!$Q$12,-8,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>4194304</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="5"/>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="5"/>
-        <v>4194304</v>
+        <v>0</v>
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="5"/>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="B90">
         <f>Layout!N2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C90">
         <v>3</v>
@@ -5790,7 +5790,7 @@
       </c>
       <c r="F90">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8388608</v>
       </c>
       <c r="G90">
         <f t="shared" si="5"/>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="H90">
         <f t="shared" si="5"/>
-        <v>8388608</v>
+        <v>0</v>
       </c>
       <c r="I90">
         <f t="shared" si="5"/>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="B91">
         <f ca="1">OFFSET(Layout!$N$2,0,-1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>3</v>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>16777216</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="5"/>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="H91">
         <f t="shared" ca="1" si="5"/>
-        <v>16777216</v>
+        <v>0</v>
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="5"/>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="B92">
         <f ca="1">OFFSET(Layout!$N$2,0,-2)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -5868,7 +5868,7 @@
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>33554432</v>
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="5"/>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="5"/>
-        <v>33554432</v>
+        <v>0</v>
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="5"/>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="B93">
         <f ca="1">OFFSET(Layout!$N$2,0,-3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C93">
         <v>3</v>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>67108864</v>
       </c>
       <c r="G93">
         <f t="shared" ca="1" si="5"/>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="H93">
         <f t="shared" ca="1" si="5"/>
-        <v>67108864</v>
+        <v>0</v>
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="5"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="B94">
         <f ca="1">OFFSET(Layout!$N$2,0,-4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C94">
         <v>3</v>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>134217728</v>
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="5"/>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="5"/>
-        <v>134217728</v>
+        <v>0</v>
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="5"/>
@@ -5975,7 +5975,7 @@
       </c>
       <c r="B95">
         <f ca="1">OFFSET(Layout!$N$2,0,-5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C95">
         <v>3</v>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>268435456</v>
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="5"/>
@@ -5993,7 +5993,7 @@
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="5"/>
-        <v>268435456</v>
+        <v>0</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="5"/>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="B96">
         <f ca="1">OFFSET(Layout!$N$2,0,-6)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C96">
         <v>3</v>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>536870912</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="5"/>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="5"/>
-        <v>536870912</v>
+        <v>0</v>
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="5"/>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="B97">
         <f ca="1">OFFSET(Layout!$N$2,0,-7)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>3</v>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1073741824</v>
       </c>
       <c r="G97">
         <f t="shared" ca="1" si="5"/>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="5"/>
-        <v>1073741824</v>
+        <v>0</v>
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="5"/>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="B98">
         <f ca="1">OFFSET(Layout!$N$2,0,-8)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>3</v>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>2147483648</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="5"/>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="5"/>
-        <v>2147483648</v>
+        <v>0</v>
       </c>
       <c r="I98">
         <f t="shared" ca="1" si="5"/>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="B99">
         <f ca="1">OFFSET(Layout!$N$2,0,-9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C99">
         <v>4</v>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99">
         <f t="shared" ca="1" si="5"/>
@@ -6149,7 +6149,7 @@
       </c>
       <c r="H99">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="5"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="B100">
         <f ca="1">OFFSET(Layout!$N$2,0,-10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -6180,7 +6180,7 @@
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="5"/>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="H100">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I100">
         <f t="shared" ca="1" si="5"/>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="B101">
         <f ca="1">OFFSET(Layout!$N$2,0,-11)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -6219,7 +6219,7 @@
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G101">
         <f t="shared" ca="1" si="5"/>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="5"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="B102">
         <f ca="1">OFFSET(Layout!$N$2,0,-12)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -6258,7 +6258,7 @@
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G102">
         <f t="shared" ca="1" si="5"/>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="H102">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I102">
         <f t="shared" ca="1" si="5"/>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="B103">
         <f>Layout!A4</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C103">
         <v>4</v>
@@ -6297,7 +6297,7 @@
       </c>
       <c r="F103">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G103">
         <f t="shared" si="5"/>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="H103">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I103">
         <f t="shared" si="5"/>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="B104">
         <f ca="1">OFFSET(Layout!$A$4,2,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C104">
         <v>4</v>
@@ -6336,7 +6336,7 @@
       </c>
       <c r="F104">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G104">
         <f t="shared" ca="1" si="5"/>
@@ -6344,7 +6344,7 @@
       </c>
       <c r="H104">
         <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="I104">
         <f t="shared" ca="1" si="5"/>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="B105">
         <f ca="1">OFFSET(Layout!$A$4,4,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C105">
         <v>4</v>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="F105">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G105">
         <f t="shared" ca="1" si="5"/>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="H105">
         <f t="shared" ca="1" si="5"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="I105">
         <f t="shared" ca="1" si="5"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="B106">
         <f ca="1">OFFSET(Layout!$A$4,6,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C106">
         <v>4</v>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="F106">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="G106">
         <f t="shared" ca="1" si="5"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="H106">
         <f t="shared" ca="1" si="5"/>
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="I106">
         <f t="shared" ca="1" si="5"/>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="B107">
         <f ca="1">OFFSET(Layout!$A$4,8,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C107">
         <v>4</v>
@@ -6453,7 +6453,7 @@
       </c>
       <c r="F107">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="G107">
         <f t="shared" ca="1" si="5"/>
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H107">
         <f t="shared" ca="1" si="5"/>
-        <v>256</v>
+        <v>0</v>
       </c>
       <c r="I107">
         <f t="shared" ca="1" si="5"/>
@@ -6500,8 +6500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F1FBC6-0864-0145-9FA6-4A5CBA82821E}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6536,23 +6536,23 @@
       </c>
       <c r="B2">
         <f ca="1">SUM(Calcs!F$3:F$34)</f>
-        <v>3221716992</v>
+        <v>1073774593</v>
       </c>
       <c r="C2">
         <f ca="1">SUM(Calcs!F$35:F$66)</f>
-        <v>16838659</v>
+        <v>4253029376</v>
       </c>
       <c r="D2">
         <f ca="1">SUM(Calcs!F$67:F$98)</f>
-        <v>7</v>
+        <v>4294967295</v>
       </c>
       <c r="E2">
         <f ca="1">SUM(Calcs!F$99:F$107)</f>
-        <v>0</v>
+        <v>511</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">_xlfn.CONCAT(".id0 = ", B2, ", .id1 = ", C2, ", .id2 = ", D2, ", .id3 = ", E2)</f>
-        <v>.id0 = 3221716992, .id1 = 16838659, .id2 = 7, .id3 = 0</v>
+        <v>.id0 = 1073774593, .id1 = 4253029376, .id2 = 4294967295, .id3 = 511</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -6561,11 +6561,11 @@
       </c>
       <c r="B3">
         <f ca="1">SUM(Calcs!G$3:G$34)</f>
-        <v>738205695</v>
+        <v>1006665726</v>
       </c>
       <c r="C3">
         <f ca="1">SUM(Calcs!G$35:G$66)</f>
-        <v>1912604672</v>
+        <v>40897280</v>
       </c>
       <c r="D3">
         <f ca="1">SUM(Calcs!G$67:G$98)</f>
@@ -6577,7 +6577,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G7" ca="1" si="0">_xlfn.CONCAT(".id0 = ", B3, ", .id1 = ", C3, ", .id2 = ", D3, ", .id3 = ", E3)</f>
-        <v>.id0 = 738205695, .id1 = 1912604672, .id2 = 0, .id3 = 0</v>
+        <v>.id0 = 1006665726, .id1 = 40897280, .id2 = 0, .id3 = 0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6586,23 +6586,23 @@
       </c>
       <c r="B4">
         <f ca="1">SUM(Calcs!H$3:H$34)</f>
-        <v>0</v>
+        <v>2214526976</v>
       </c>
       <c r="C4">
         <f ca="1">SUM(Calcs!H$35:H$66)</f>
-        <v>0</v>
+        <v>1040639</v>
       </c>
       <c r="D4">
         <f ca="1">SUM(Calcs!H$67:H$98)</f>
-        <v>4294967288</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f ca="1">SUM(Calcs!H$99:H$107)</f>
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>.id0 = 0, .id1 = 0, .id2 = 4294967288, .id3 = 511</v>
+        <v>.id0 = 2214526976, .id1 = 1040639, .id2 = 0, .id3 = 0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6615,7 +6615,7 @@
       </c>
       <c r="C5">
         <f ca="1">SUM(Calcs!I$35:I$66)</f>
-        <v>2147484672</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f ca="1">SUM(Calcs!I$67:I$98)</f>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>.id0 = 0, .id1 = 2147484672, .id2 = 0, .id3 = 0</v>
+        <v>.id0 = 0, .id1 = 0, .id2 = 0, .id3 = 0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6636,11 +6636,11 @@
       </c>
       <c r="B6">
         <f ca="1">SUM(Calcs!J$3:J$34)</f>
-        <v>335044608</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f ca="1">SUM(Calcs!J$35:J$66)</f>
-        <v>218039292</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f ca="1">SUM(Calcs!J$67:J$98)</f>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>.id0 = 335044608, .id1 = 218039292, .id2 = 0, .id3 = 0</v>
+        <v>.id0 = 0, .id1 = 0, .id2 = 0, .id3 = 0</v>
       </c>
     </row>
     <row r="7" spans="1:7">

</xml_diff>